<commit_message>
Converted files and OpenAPI changes for 2.14.5
</commit_message>
<xml_diff>
--- a/converted_files/837/837I-all-fields.xlsx
+++ b/converted_files/837/837I-all-fields.xlsx
@@ -1875,7 +1875,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>690148897e79911955eafc2b</t>
+          <t>6918d0577f059d7aab1b4db1</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -3224,7 +3224,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>690148897e79911955eafc2b</t>
+          <t>6918d0577f059d7aab1b4db1</t>
         </is>
       </c>
       <c r="B3"/>

</xml_diff>